<commit_message>
Prototype - translation controls
</commit_message>
<xml_diff>
--- a/planning/time_plan.xlsx
+++ b/planning/time_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cm3070\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4BBC58-B4BE-4235-89CC-9983F0AFDEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E19B9C-30C6-4CC0-BD1E-C7CBBAC1AF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="3120" windowWidth="28020" windowHeight="15910" xr2:uid="{D62AB7A3-E81C-4FB7-B857-FBF7D3950652}"/>
+    <workbookView xWindow="-38510" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{D62AB7A3-E81C-4FB7-B857-FBF7D3950652}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,6 +662,9 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
+      <c r="D14" s="1">
+        <v>45249</v>
+      </c>
       <c r="E14">
         <v>0.5</v>
       </c>

</xml_diff>

<commit_message>
alpha 0.2: piece deck, spawning
</commit_message>
<xml_diff>
--- a/planning/time_plan.xlsx
+++ b/planning/time_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cm3070\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E19B9C-30C6-4CC0-BD1E-C7CBBAC1AF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540677E5-2E20-4B76-93F0-A778B1DEB479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{D62AB7A3-E81C-4FB7-B857-FBF7D3950652}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Junk art</t>
   </si>
@@ -77,15 +77,6 @@
     <t>Topic 7 checklist</t>
   </si>
   <si>
-    <t>Topic 8 checklist</t>
-  </si>
-  <si>
-    <t>Topic 9 checklist</t>
-  </si>
-  <si>
-    <t>Topic 10 checklist</t>
-  </si>
-  <si>
     <t>Exam</t>
   </si>
   <si>
@@ -120,6 +111,18 @@
   </si>
   <si>
     <t>Extend evaluations</t>
+  </si>
+  <si>
+    <t>Submit draft report (Feb 12)</t>
+  </si>
+  <si>
+    <t>Topic 8 checklist (Jan 29)</t>
+  </si>
+  <si>
+    <t>Topic 9 checklist (Feb 12)</t>
+  </si>
+  <si>
+    <t>Topic 10 checklist (Feb 26)</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9C2678-9EC5-414D-A01F-1C989404219A}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -525,7 +528,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>45214</v>
@@ -539,7 +542,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1">
         <v>45215</v>
@@ -553,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1">
         <v>45216</v>
@@ -584,7 +587,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1">
         <v>45220</v>
@@ -598,7 +601,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1">
         <v>45222</v>
@@ -612,7 +615,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
         <v>45226</v>
@@ -643,7 +646,7 @@
         <v>0.1</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1">
         <v>45228</v>
@@ -679,6 +682,9 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
+      <c r="D15" s="1">
+        <v>45261</v>
+      </c>
       <c r="E15">
         <v>0.5</v>
       </c>
@@ -693,6 +699,9 @@
       <c r="C16" t="s">
         <v>10</v>
       </c>
+      <c r="D16" s="1">
+        <v>45280</v>
+      </c>
       <c r="E16">
         <v>0.5</v>
       </c>
@@ -705,7 +714,10 @@
         <v>0.1</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45280</v>
       </c>
       <c r="E17">
         <v>10</v>
@@ -721,6 +733,9 @@
       <c r="C18" t="s">
         <v>11</v>
       </c>
+      <c r="D18" s="1">
+        <v>44927</v>
+      </c>
       <c r="E18">
         <v>0.5</v>
       </c>
@@ -735,6 +750,9 @@
       <c r="C19" t="s">
         <v>12</v>
       </c>
+      <c r="D19" s="1">
+        <v>44934</v>
+      </c>
       <c r="E19">
         <v>0.5</v>
       </c>
@@ -747,7 +765,7 @@
         <v>0.1</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E20">
         <v>0.5</v>
@@ -761,7 +779,7 @@
         <v>0.1</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E21">
         <v>0.5</v>
@@ -769,30 +787,30 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>0.1</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>0.1</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E23">
-        <v>60</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -803,10 +821,10 @@
         <v>0.1</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -814,12 +832,26 @@
         <v>22</v>
       </c>
       <c r="B25">
+        <v>0.1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
         <v>1</v>
       </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25">
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
beta 0.6 webgl build
</commit_message>
<xml_diff>
--- a/planning/time_plan.xlsx
+++ b/planning/time_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cm3070\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37B03B3-FF86-4E65-9D55-047E24EAF274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1FFC11-44FA-4FF3-A2DC-38FBC7480E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{D62AB7A3-E81C-4FB7-B857-FBF7D3950652}"/>
   </bookViews>
@@ -194,9 +194,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -234,7 +234,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -340,7 +340,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -482,7 +482,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -493,7 +493,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -896,6 +896,9 @@
       <c r="C22" t="s">
         <v>25</v>
       </c>
+      <c r="D22" s="1">
+        <v>45333</v>
+      </c>
       <c r="E22">
         <v>0</v>
       </c>
@@ -914,12 +917,18 @@
       <c r="C23" t="s">
         <v>28</v>
       </c>
+      <c r="D23" s="1">
+        <v>45333</v>
+      </c>
       <c r="E23">
         <v>0.5</v>
+      </c>
+      <c r="F23">
+        <v>100</v>
       </c>
       <c r="G23">
         <f>F23/100*E23</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -979,7 +988,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G27" s="2">
         <f>SUM(G4:G26)</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final report evaluation section
</commit_message>
<xml_diff>
--- a/planning/time_plan.xlsx
+++ b/planning/time_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cm3070\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1FFC11-44FA-4FF3-A2DC-38FBC7480E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87066382-D518-40B3-97EE-A8965A17021C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="37690" windowHeight="21820" xr2:uid="{D62AB7A3-E81C-4FB7-B857-FBF7D3950652}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37580" windowHeight="21820" xr2:uid="{D62AB7A3-E81C-4FB7-B857-FBF7D3950652}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Junk art</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Weighted</t>
+  </si>
+  <si>
+    <t>Weight of CWK</t>
+  </si>
+  <si>
+    <t>CWK</t>
   </si>
 </sst>
 </file>
@@ -490,24 +496,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D9C2678-9EC5-414D-A01F-1C989404219A}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="49.08984375" customWidth="1"/>
     <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -524,13 +531,19 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -541,7 +554,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -555,7 +568,7 @@
         <v>45214</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -569,7 +582,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -583,7 +596,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
@@ -600,14 +613,21 @@
         <v>0.5</v>
       </c>
       <c r="F8">
+        <v>0.625</v>
+      </c>
+      <c r="G8">
         <v>100</v>
       </c>
-      <c r="G8">
-        <f>F8/100*E8</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <f>G8/100*E8</f>
+        <v>0.5</v>
+      </c>
+      <c r="I8">
+        <f>F8*G8/100</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -621,7 +641,7 @@
         <v>45220</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4</v>
       </c>
@@ -635,7 +655,7 @@
         <v>45222</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4</v>
       </c>
@@ -649,7 +669,7 @@
         <v>45226</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4</v>
       </c>
@@ -666,14 +686,21 @@
         <v>0.5</v>
       </c>
       <c r="F12">
+        <v>0.625</v>
+      </c>
+      <c r="G12">
         <v>100</v>
       </c>
-      <c r="G12">
-        <f t="shared" ref="G12:G21" si="0">F12/100*E12</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <f t="shared" ref="H12:H21" si="0">G12/100*E12</f>
+        <v>0.5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I25" si="1">F12*G12/100</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>4</v>
       </c>
@@ -686,18 +713,11 @@
       <c r="D13" s="1">
         <v>45228</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="G13">
         <v>64</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6</v>
       </c>
@@ -714,14 +734,21 @@
         <v>0.5</v>
       </c>
       <c r="F14">
+        <v>0.625</v>
+      </c>
+      <c r="G14">
         <v>100</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>8</v>
       </c>
@@ -738,14 +765,21 @@
         <v>0.5</v>
       </c>
       <c r="F15">
+        <v>0.625</v>
+      </c>
+      <c r="G15">
         <v>100</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>10</v>
       </c>
@@ -762,14 +796,21 @@
         <v>0.5</v>
       </c>
       <c r="F16">
+        <v>0.625</v>
+      </c>
+      <c r="G16">
         <v>100</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>10</v>
       </c>
@@ -785,12 +826,22 @@
       <c r="E17">
         <v>10</v>
       </c>
+      <c r="F17">
+        <v>12.5</v>
+      </c>
       <c r="G17">
+        <v>69</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>6.8999999999999995</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>8.625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>12</v>
       </c>
@@ -807,14 +858,21 @@
         <v>0.5</v>
       </c>
       <c r="F18">
+        <v>0.625</v>
+      </c>
+      <c r="G18">
         <v>100</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>14</v>
       </c>
@@ -831,14 +889,21 @@
         <v>0.5</v>
       </c>
       <c r="F19">
+        <v>0.625</v>
+      </c>
+      <c r="G19">
         <v>100</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>16</v>
       </c>
@@ -855,14 +920,21 @@
         <v>0.5</v>
       </c>
       <c r="F20">
+        <v>0.625</v>
+      </c>
+      <c r="G20">
         <v>100</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>18</v>
       </c>
@@ -879,14 +951,21 @@
         <v>0.5</v>
       </c>
       <c r="F21">
+        <v>0.625</v>
+      </c>
+      <c r="G21">
         <v>100</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>19</v>
       </c>
@@ -899,15 +978,8 @@
       <c r="D22" s="1">
         <v>45333</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <f t="shared" ref="G22" si="1">F22/100*E22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20</v>
       </c>
@@ -924,14 +996,21 @@
         <v>0.5</v>
       </c>
       <c r="F23">
+        <v>0.625</v>
+      </c>
+      <c r="G23">
         <v>100</v>
       </c>
-      <c r="G23">
-        <f>F23/100*E23</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <f>G23/100*E23</f>
+        <v>0.5</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -944,12 +1023,19 @@
       <c r="E24">
         <v>60</v>
       </c>
-      <c r="G24">
-        <f>F24/100*E24</f>
+      <c r="F24">
+        <v>75</v>
+      </c>
+      <c r="H24">
+        <f>G24/100*E24</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>22</v>
       </c>
@@ -962,12 +1048,19 @@
       <c r="E25">
         <v>5</v>
       </c>
-      <c r="G25">
-        <f>F25/100*E25</f>
+      <c r="F25">
+        <v>6.25</v>
+      </c>
+      <c r="H25">
+        <f>G25/100*E25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>22</v>
       </c>
@@ -980,15 +1073,19 @@
       <c r="E26">
         <v>20</v>
       </c>
-      <c r="G26">
-        <f>F26/100*E26</f>
+      <c r="H26">
+        <f>G26/100*E26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G27" s="2">
-        <f>SUM(G4:G26)</f>
-        <v>5</v>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H27" s="2">
+        <f>SUM(H4:H26)</f>
+        <v>11.899999999999999</v>
+      </c>
+      <c r="I27">
+        <f>SUM(I8:I26)</f>
+        <v>14.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>